<commit_message>
bunch of work related to mode choices and transit
</commit_message>
<xml_diff>
--- a/2021/analysis_in_progress/seattle_sector_mode_share/trips_by_mode_pm_seattle_od.xlsx
+++ b/2021/analysis_in_progress/seattle_sector_mode_share/trips_by_mode_pm_seattle_od.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\travel-studies\2021\analysis_in_progress\seattle_sector_mode_share\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43EB9EA7-CD8F-49FA-9BEB-96A312A6852C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98718F0-4C92-4B12-AD3A-47684BD65F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="trips_by_mode_pm_seattle_od" sheetId="1" r:id="rId1"/>
+    <sheet name="compare_targets" sheetId="2" r:id="rId1"/>
+    <sheet name="trips_by_mode_pm_seattle_od" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="36">
   <si>
     <t>survey</t>
   </si>
@@ -87,11 +100,53 @@
   <si>
     <t>West Seattle</t>
   </si>
+  <si>
+    <t>PM Trips</t>
+  </si>
+  <si>
+    <t>PM Trips MOE</t>
+  </si>
+  <si>
+    <t>if we can only measure +/- 10% essentially; the targets should be that way?</t>
+  </si>
+  <si>
+    <t>2035 Target</t>
+  </si>
+  <si>
+    <t>PM Peak vs all day</t>
+  </si>
+  <si>
+    <t>so much HOV; Consider driving non-driving</t>
+  </si>
+  <si>
+    <t>help communicate to Seattle; Fehr and Peers</t>
+  </si>
+  <si>
+    <t>What can the city do to promote this goal or hinder it?</t>
+  </si>
+  <si>
+    <t>2017/2019 moe</t>
+  </si>
+  <si>
+    <t>Origin or Only Dest Sector</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>options- could aggregate geography</t>
+  </si>
+  <si>
+    <t>2017/2019 sample size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017/2019 share estimate </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -632,6 +687,1146 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>SOV PM Peak Mode Share: 2017/2019 vs </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>2035 Seattle Comp Plan Target</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>compare_targets!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2017/2019 share estimate </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>compare_targets!$G$2:$G$9</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>9.3089430801856304E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.99662156576872E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.13150837500048099</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.14536480836135399</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8.2668853612588994E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8.0077024514336903E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>8.8143566572321794E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.14056209514207799</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>compare_targets!$G$2:$G$9</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>9.3089430801856304E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.99662156576872E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.13150837500048099</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.14536480836135399</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8.2668853612588994E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8.0077024514336903E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>8.8143566572321794E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.14056209514207799</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>compare_targets!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Capitol Hill/Central District</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Downtown/Lake Union</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Duwamish</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Magnolia/Queen Anne</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Northeast Seattle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Northwest Seattle</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Southeast Seattle</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>West Seattle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>compare_targets!$E$2:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.37981220118725001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25233229899214699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63235859663195604</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34249604838703901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35824800601696599</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.335077362803891</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.29314712194824599</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.41883518966959699</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AFBC-4498-A6F2-486F3B82206A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>compare_targets!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2035 Target</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>compare_targets!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Capitol Hill/Central District</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Downtown/Lake Union</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Duwamish</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Magnolia/Queen Anne</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Northeast Seattle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Northwest Seattle</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Southeast Seattle</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>West Seattle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>compare_targets!$F$2:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AFBC-4498-A6F2-486F3B82206A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1697635216"/>
+        <c:axId val="1697635632"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1697635216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1697635632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1697635632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1697635216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C7AE7AE-D5FF-05BC-1354-07C6AB089D66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -928,11 +2123,311 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888FD444-2E45-4D6F-AC62-FDA4D3DAF291}">
+  <dimension ref="A1:L24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>46022.060839439</v>
+      </c>
+      <c r="D2">
+        <v>16882.5466800266</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.37981220118725001</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G2" s="1">
+        <v>9.3089430801856304E-2</v>
+      </c>
+      <c r="H2">
+        <v>416</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>69735.4954153453</v>
+      </c>
+      <c r="D3">
+        <v>20402.600677124399</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.25233229899214699</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5.99662156576872E-2</v>
+      </c>
+      <c r="H3">
+        <v>533</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>38754.433670037797</v>
+      </c>
+      <c r="D4">
+        <v>13957.080463362799</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.63235859663195604</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.13150837500048099</v>
+      </c>
+      <c r="H4">
+        <v>234</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>28417.6385878562</v>
+      </c>
+      <c r="D5">
+        <v>13857.295340479601</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.34249604838703901</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.14536480836135399</v>
+      </c>
+      <c r="H5">
+        <v>185</v>
+      </c>
+      <c r="J5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>84822.011010532602</v>
+      </c>
+      <c r="D6">
+        <v>27295.762459762002</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.35824800601696599</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="G6" s="1">
+        <v>8.2668853612588994E-2</v>
+      </c>
+      <c r="H6">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>65047.392623025997</v>
+      </c>
+      <c r="D7">
+        <v>19037.696412416899</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.335077362803891</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.37</v>
+      </c>
+      <c r="G7" s="1">
+        <v>8.0077024514336903E-2</v>
+      </c>
+      <c r="H7">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>24678.1722544738</v>
+      </c>
+      <c r="D8">
+        <v>9207.4335669502907</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.29314712194824599</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="G8" s="1">
+        <v>8.8143566572321794E-2</v>
+      </c>
+      <c r="H8">
+        <v>321</v>
+      </c>
+      <c r="L8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>43609.079619103897</v>
+      </c>
+      <c r="D9">
+        <v>21268.91580101</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.41883518966959699</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.14056209514207799</v>
+      </c>
+      <c r="H9">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -980,256 +2475,256 @@
         <v>10</v>
       </c>
       <c r="E2">
-        <v>34348.588976154097</v>
+        <v>27577.074914832701</v>
       </c>
       <c r="F2">
-        <v>6430.3969439791299</v>
+        <v>6081.0805024811698</v>
       </c>
       <c r="G2" s="1">
-        <v>0.233750780168379</v>
+        <v>0.22758888530112101</v>
       </c>
       <c r="H2" s="1">
-        <v>4.5927601263276399E-2</v>
+        <v>5.3012529295830203E-2</v>
       </c>
       <c r="I2">
-        <v>484</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>39118.601507781001</v>
+        <v>49030.580683298198</v>
       </c>
       <c r="F3">
-        <v>7568.7485477791297</v>
+        <v>14495.7697426128</v>
       </c>
       <c r="G3" s="1">
-        <v>0.26621191420374701</v>
+        <v>0.177413225087867</v>
       </c>
       <c r="H3" s="1">
-        <v>5.1509846392159997E-2</v>
+        <v>4.7103087799006599E-2</v>
       </c>
       <c r="I3">
-        <v>868</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>611.74626292265202</v>
+        <v>14180.4666869351</v>
       </c>
       <c r="F4">
-        <v>275.23084527594398</v>
+        <v>9450.1747506729498</v>
       </c>
       <c r="G4" s="1">
-        <v>4.1630870578856201E-3</v>
+        <v>0.231383590586933</v>
       </c>
       <c r="H4" s="1">
-        <v>1.9558704129718002E-3</v>
+        <v>0.13012858697736199</v>
       </c>
       <c r="I4">
-        <v>40</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E5">
-        <v>52359.1830021227</v>
+        <v>15692.9006072509</v>
       </c>
       <c r="F5">
-        <v>17017.8393410668</v>
+        <v>10128.1753533881</v>
       </c>
       <c r="G5" s="1">
-        <v>0.35631739877937302</v>
+        <v>0.18913452041756901</v>
       </c>
       <c r="H5" s="1">
-        <v>7.9892446140797393E-2</v>
+        <v>0.114148888965919</v>
       </c>
       <c r="I5">
-        <v>532</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E6">
-        <v>20232.592031691998</v>
+        <v>89112.057829221798</v>
       </c>
       <c r="F6">
-        <v>6359.5090397412296</v>
+        <v>20444.689231650598</v>
       </c>
       <c r="G6" s="1">
-        <v>0.13768787345296199</v>
+        <v>0.37636713217543399</v>
       </c>
       <c r="H6" s="1">
-        <v>4.16611946061477E-2</v>
+        <v>7.2299286791472503E-2</v>
       </c>
       <c r="I6">
-        <v>372</v>
+        <v>421</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7">
-        <v>57374.871862704204</v>
+        <v>87297.423754793999</v>
       </c>
       <c r="F7">
-        <v>15207.576952229399</v>
+        <v>25732.361060643601</v>
       </c>
       <c r="G7" s="1">
-        <v>0.17369025200469501</v>
+        <v>0.44969351347951603</v>
       </c>
       <c r="H7" s="1">
-        <v>4.1445340653997902E-2</v>
+        <v>8.7162907796983394E-2</v>
       </c>
       <c r="I7">
-        <v>494</v>
+        <v>593</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8">
-        <v>85182.982593162305</v>
+        <v>43898.481021574102</v>
       </c>
       <c r="F8">
-        <v>13932.220030897</v>
+        <v>10745.5157579806</v>
       </c>
       <c r="G8" s="1">
-        <v>0.25787340751754301</v>
+        <v>0.52146136418353195</v>
       </c>
       <c r="H8" s="1">
-        <v>3.9970019740884898E-2</v>
+        <v>9.0599464563873994E-2</v>
       </c>
       <c r="I8">
-        <v>1875</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E9">
-        <v>2238.0933853817401</v>
+        <v>43524.017326369001</v>
       </c>
       <c r="F9">
-        <v>1062.39744563975</v>
+        <v>18173.8414530708</v>
       </c>
       <c r="G9" s="1">
-        <v>6.7753528939850701E-3</v>
+        <v>0.41801822490394402</v>
       </c>
       <c r="H9" s="1">
-        <v>3.2732660338762802E-3</v>
+        <v>0.13389902974163101</v>
       </c>
       <c r="I9">
-        <v>71</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E10">
-        <v>87250.298839035095</v>
+        <v>29807.505068603499</v>
       </c>
       <c r="F10">
-        <v>22428.213139282601</v>
+        <v>7069.6845745720602</v>
       </c>
       <c r="G10" s="1">
-        <v>0.26413176885346501</v>
+        <v>0.245996244094844</v>
       </c>
       <c r="H10" s="1">
-        <v>5.4285637528548598E-2</v>
+        <v>5.8388125936883702E-2</v>
       </c>
       <c r="I10">
-        <v>659</v>
+        <v>609</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -1238,27 +2733,27 @@
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E11">
-        <v>97390.290145711697</v>
+        <v>71766.0965874822</v>
       </c>
       <c r="F11">
-        <v>16428.060389825299</v>
+        <v>13668.781366753999</v>
       </c>
       <c r="G11" s="1">
-        <v>0.29482844125033902</v>
+        <v>0.25967986652643699</v>
       </c>
       <c r="H11" s="1">
-        <v>4.4458117863772503E-2</v>
+        <v>4.6096348234533797E-2</v>
       </c>
       <c r="I11">
-        <v>1597</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -1267,259 +2762,259 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12">
-        <v>15572.503723768101</v>
+        <v>2994.6795361941599</v>
       </c>
       <c r="F12">
-        <v>9476.8868396767994</v>
+        <v>1795.3725303041799</v>
       </c>
       <c r="G12" s="1">
-        <v>0.224351417110047</v>
+        <v>4.8864379363496198E-2</v>
       </c>
       <c r="H12" s="1">
-        <v>0.116272690132725</v>
+        <v>3.0983226503520599E-2</v>
       </c>
       <c r="I12">
-        <v>164</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
       <c r="E13">
-        <v>3419.2651083863202</v>
+        <v>31045.231042994201</v>
       </c>
       <c r="F13">
-        <v>1828.7794973053101</v>
+        <v>20015.755720801801</v>
       </c>
       <c r="G13" s="1">
-        <v>4.9260991433931499E-2</v>
+        <v>0.37416440921420901</v>
       </c>
       <c r="H13" s="1">
-        <v>2.7967683439892501E-2</v>
+        <v>0.17139846382275101</v>
       </c>
       <c r="I13">
-        <v>62</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14">
-        <v>637.32490576641601</v>
+        <v>30018.178455125701</v>
       </c>
       <c r="F14">
-        <v>734.40271430050097</v>
+        <v>5574.6111318416197</v>
       </c>
       <c r="G14" s="1">
-        <v>9.1818726329785192E-3</v>
+        <v>0.126782570322164</v>
       </c>
       <c r="H14" s="1">
-        <v>1.0738964306414101E-2</v>
+        <v>2.8263106110412099E-2</v>
       </c>
       <c r="I14">
-        <v>5</v>
+        <v>626</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E15">
-        <v>44715.7957182221</v>
+        <v>23430.046116510999</v>
       </c>
       <c r="F15">
-        <v>14580.0508953525</v>
+        <v>3754.89835440039</v>
       </c>
       <c r="G15" s="1">
-        <v>0.64421574812499105</v>
+        <v>0.12069473881286601</v>
       </c>
       <c r="H15" s="1">
-        <v>0.118207011467396</v>
+        <v>2.6552556050287501E-2</v>
       </c>
       <c r="I15">
-        <v>281</v>
+        <v>480</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E16">
-        <v>5003.2270589949903</v>
+        <v>8333.5912940574399</v>
       </c>
       <c r="F16">
-        <v>1893.0917637861301</v>
+        <v>3668.1186345698302</v>
       </c>
       <c r="G16" s="1">
-        <v>7.20809640324971E-2</v>
+        <v>9.8993080936251907E-2</v>
       </c>
       <c r="H16" s="1">
-        <v>3.116871364966E-2</v>
+        <v>4.2951429941325101E-2</v>
       </c>
       <c r="I16">
-        <v>93</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E17">
-        <v>49621.526443158698</v>
+        <v>13994.9117089759</v>
       </c>
       <c r="F17">
-        <v>32396.882493129298</v>
+        <v>4165.3695778942802</v>
       </c>
       <c r="G17" s="1">
-        <v>0.37691441706740603</v>
+        <v>0.134411493001801</v>
       </c>
       <c r="H17" s="1">
-        <v>0.17279604135162399</v>
+        <v>5.0087810622864402E-2</v>
       </c>
       <c r="I17">
-        <v>133</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18">
-        <v>38254.034513404396</v>
+        <v>224.792945636235</v>
       </c>
       <c r="F18">
-        <v>22708.320523227801</v>
+        <v>125.79165529513401</v>
       </c>
       <c r="G18" s="1">
-        <v>0.29056939906136497</v>
+        <v>1.85517775467147E-3</v>
       </c>
       <c r="H18" s="1">
-        <v>0.14611406451734901</v>
+        <v>1.0814320162868499E-3</v>
       </c>
       <c r="I18">
-        <v>136</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
       <c r="E19">
-        <v>4841.1078506327804</v>
+        <v>1284.83986746041</v>
       </c>
       <c r="F19">
-        <v>5199.6001124591203</v>
+        <v>736.21113341880096</v>
       </c>
       <c r="G19" s="1">
-        <v>3.6772011549702402E-2</v>
+        <v>4.6490900460672601E-3</v>
       </c>
       <c r="H19" s="1">
-        <v>3.9844020294891397E-2</v>
+        <v>2.70853906538337E-3</v>
       </c>
       <c r="I19">
-        <v>13</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20">
-        <v>35379.295074190697</v>
+        <v>637.32490576641601</v>
       </c>
       <c r="F20">
-        <v>15123.806068657001</v>
+        <v>734.398537402957</v>
       </c>
       <c r="G20" s="1">
-        <v>0.26873349803979701</v>
+        <v>1.0399271640515E-2</v>
       </c>
       <c r="H20" s="1">
-        <v>0.11707303191251001</v>
+        <v>1.22073531808363E-2</v>
       </c>
       <c r="I20">
-        <v>235</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -1528,27 +3023,27 @@
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E21">
-        <v>3498.0792013547598</v>
+        <v>4782.4925040020998</v>
       </c>
       <c r="F21">
-        <v>1463.48081804352</v>
+        <v>5199.0425734831197</v>
       </c>
       <c r="G21" s="1">
-        <v>2.6570655470354299E-2</v>
+        <v>5.76397218578645E-2</v>
       </c>
       <c r="H21" s="1">
-        <v>1.38332715289178E-2</v>
+        <v>6.1834836386254602E-2</v>
       </c>
       <c r="I21">
-        <v>60</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -1557,259 +3052,259 @@
         <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E22">
-        <v>119713.611447626</v>
+        <v>139.886036193005</v>
       </c>
       <c r="F22">
-        <v>23785.920561827199</v>
+        <v>136.309109245418</v>
       </c>
       <c r="G22" s="1">
-        <v>0.39947212456362202</v>
+        <v>5.9081237215111897E-4</v>
       </c>
       <c r="H22" s="1">
-        <v>6.4601794651534303E-2</v>
+        <v>5.8259566519519405E-4</v>
       </c>
       <c r="I22">
-        <v>565</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E23">
-        <v>50352.696055336601</v>
+        <v>789.57812969211204</v>
       </c>
       <c r="F23">
-        <v>12484.4759869432</v>
+        <v>505.26980952423497</v>
       </c>
       <c r="G23" s="1">
-        <v>0.16802181662969501</v>
+        <v>4.0673383936869296E-3</v>
       </c>
       <c r="H23" s="1">
-        <v>4.0840101936613797E-2</v>
+        <v>2.68295751343636E-3</v>
       </c>
       <c r="I23">
-        <v>828</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
       </c>
       <c r="E24">
-        <v>236.49664680625401</v>
+        <v>251.75937778004501</v>
       </c>
       <c r="F24">
-        <v>168.07408737741599</v>
+        <v>178.12140110893299</v>
       </c>
       <c r="G24" s="1">
-        <v>7.8916521529549203E-4</v>
+        <v>2.99059980045005E-3</v>
       </c>
       <c r="H24" s="1">
-        <v>5.7048055131093598E-4</v>
+        <v>2.1781517827362102E-3</v>
       </c>
       <c r="I24">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25">
-        <v>94891.471792890996</v>
+        <v>147.25713413107499</v>
       </c>
       <c r="F25">
-        <v>27713.6237049138</v>
+        <v>236.93559768304701</v>
       </c>
       <c r="G25" s="1">
-        <v>0.31664317350127802</v>
+        <v>1.4143034029310501E-3</v>
       </c>
       <c r="H25" s="1">
-        <v>7.0457361712859295E-2</v>
+        <v>2.3047771125553301E-3</v>
       </c>
       <c r="I25">
-        <v>712</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E26">
-        <v>34161.632746788797</v>
+        <v>46022.060839439</v>
       </c>
       <c r="F26">
-        <v>11892.491613165899</v>
+        <v>16882.5466800266</v>
       </c>
       <c r="G26" s="1">
-        <v>0.113993887970644</v>
+        <v>0.37981220118725001</v>
       </c>
       <c r="H26" s="1">
-        <v>3.81216533039943E-2</v>
+        <v>9.3089430801856304E-2</v>
       </c>
       <c r="I26">
-        <v>473</v>
+        <v>416</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E27">
-        <v>118558.136128559</v>
+        <v>69735.4954153453</v>
       </c>
       <c r="F27">
-        <v>28349.6286757585</v>
+        <v>20402.600677124399</v>
       </c>
       <c r="G27" s="1">
-        <v>0.45342014521581397</v>
+        <v>0.25233229899214699</v>
       </c>
       <c r="H27" s="1">
-        <v>7.1505977796151907E-2</v>
+        <v>5.99662156576872E-2</v>
       </c>
       <c r="I27">
-        <v>782</v>
+        <v>533</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E28">
-        <v>35651.645757077502</v>
+        <v>38754.433670037797</v>
       </c>
       <c r="F28">
-        <v>6548.6647453092401</v>
+        <v>13957.080463362799</v>
       </c>
       <c r="G28" s="1">
-        <v>0.13634808140731899</v>
+        <v>0.63235859663195604</v>
       </c>
       <c r="H28" s="1">
-        <v>2.8649097692518201E-2</v>
+        <v>0.13150837500048099</v>
       </c>
       <c r="I28">
-        <v>701</v>
+        <v>234</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E29">
-        <v>1246.2615556875501</v>
+        <v>28417.6385878562</v>
       </c>
       <c r="F29">
-        <v>656.79252513568599</v>
+        <v>13857.295340479601</v>
       </c>
       <c r="G29" s="1">
-        <v>4.7662700680785501E-3</v>
+        <v>0.34249604838703901</v>
       </c>
       <c r="H29" s="1">
-        <v>2.5875609041209201E-3</v>
+        <v>0.14536480836135399</v>
       </c>
       <c r="I29">
-        <v>28</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" t="s">
         <v>13</v>
       </c>
       <c r="E30">
-        <v>82444.1718059876</v>
+        <v>84822.011010532602</v>
       </c>
       <c r="F30">
-        <v>20473.0470277483</v>
+        <v>27295.762459762002</v>
       </c>
       <c r="G30" s="1">
-        <v>0.31530394769308101</v>
+        <v>0.35824800601696599</v>
       </c>
       <c r="H30" s="1">
-        <v>6.4887891003569204E-2</v>
+        <v>8.2668853612588994E-2</v>
       </c>
       <c r="I30">
-        <v>864</v>
+        <v>566</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
@@ -1818,27 +3313,27 @@
         <v>19</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E31">
-        <v>21807.869956911502</v>
+        <v>65047.392623025997</v>
       </c>
       <c r="F31">
-        <v>8146.7187383995497</v>
+        <v>19037.696412416899</v>
       </c>
       <c r="G31" s="1">
-        <v>8.3403196824789402E-2</v>
+        <v>0.335077362803891</v>
       </c>
       <c r="H31" s="1">
-        <v>3.0745780020714701E-2</v>
+        <v>8.0077024514336903E-2</v>
       </c>
       <c r="I31">
-        <v>186</v>
+        <v>664</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
@@ -1847,254 +3342,254 @@
         <v>20</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E32">
-        <v>50921.773853045197</v>
+        <v>24678.1722544738</v>
       </c>
       <c r="F32">
-        <v>11534.568071257499</v>
+        <v>9207.4335669502907</v>
       </c>
       <c r="G32" s="1">
-        <v>0.48367291397995099</v>
+        <v>0.29314712194824599</v>
       </c>
       <c r="H32" s="1">
-        <v>8.3769750160796394E-2</v>
+        <v>8.8143566572321794E-2</v>
       </c>
       <c r="I32">
-        <v>413</v>
+        <v>321</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E33">
-        <v>10051.482510604599</v>
+        <v>43609.079619103897</v>
       </c>
       <c r="F33">
-        <v>3748.5314284678302</v>
+        <v>21268.91580101</v>
       </c>
       <c r="G33" s="1">
-        <v>9.5472515347811204E-2</v>
+        <v>0.41883518966959699</v>
       </c>
       <c r="H33" s="1">
-        <v>3.5840352686582901E-2</v>
+        <v>0.14056209514207799</v>
       </c>
       <c r="I33">
-        <v>256</v>
+        <v>298</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E34">
-        <v>600.92111116205001</v>
+        <v>17415.431359890801</v>
       </c>
       <c r="F34">
-        <v>442.82442434893602</v>
+        <v>5832.5478908868799</v>
       </c>
       <c r="G34" s="1">
-        <v>5.7077600192523099E-3</v>
+        <v>0.14372657805356601</v>
       </c>
       <c r="H34" s="1">
-        <v>4.2912998117356198E-3</v>
+        <v>4.7169524645333E-2</v>
       </c>
       <c r="I34">
-        <v>16</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E35">
-        <v>35748.577892536399</v>
+        <v>83748.251120012996</v>
       </c>
       <c r="F35">
-        <v>12118.5118645732</v>
+        <v>15922.856798786601</v>
       </c>
       <c r="G35" s="1">
-        <v>0.33955256330663602</v>
+        <v>0.303036332011693</v>
       </c>
       <c r="H35" s="1">
-        <v>8.6720421897417202E-2</v>
+        <v>5.0981365516033599E-2</v>
       </c>
       <c r="I35">
-        <v>407</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
       </c>
       <c r="E36">
-        <v>7583.5476803155498</v>
+        <v>4655.5329916830497</v>
       </c>
       <c r="F36">
-        <v>4382.37982010214</v>
+        <v>1851.4558345309799</v>
       </c>
       <c r="G36" s="1">
-        <v>7.2031202515243295E-2</v>
+        <v>7.5964632440765803E-2</v>
       </c>
       <c r="H36" s="1">
-        <v>4.0378830272029202E-2</v>
+        <v>3.4965293917251297E-2</v>
       </c>
       <c r="I36">
-        <v>109</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E37">
-        <v>48808.950230335897</v>
+        <v>3009.0813579437799</v>
       </c>
       <c r="F37">
-        <v>18296.648816706002</v>
+        <v>1283.8970758185401</v>
       </c>
       <c r="G37" s="1">
-        <v>0.39025499601450803</v>
+        <v>3.6266154599181102E-2</v>
       </c>
       <c r="H37" s="1">
-        <v>0.114326579270204</v>
+        <v>1.89891932693503E-2</v>
       </c>
       <c r="I37">
-        <v>370</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D38" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E38">
-        <v>17051.404368339499</v>
+        <v>32403.057272162299</v>
       </c>
       <c r="F38">
-        <v>4503.2326865743698</v>
+        <v>11862.887608272</v>
       </c>
       <c r="G38" s="1">
-        <v>0.13633556371126901</v>
+        <v>0.136855169057054</v>
       </c>
       <c r="H38" s="1">
-        <v>4.43375861928142E-2</v>
+        <v>4.7663483548875299E-2</v>
       </c>
       <c r="I38">
-        <v>207</v>
+        <v>394</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E39">
-        <v>179.08715127534501</v>
+        <v>15948.3488113187</v>
       </c>
       <c r="F39">
-        <v>238.95648645841101</v>
+        <v>6678.3083079877097</v>
       </c>
       <c r="G39" s="1">
-        <v>1.43190245185342E-3</v>
+        <v>8.2154417652730696E-2</v>
       </c>
       <c r="H39" s="1">
-        <v>1.93721386211825E-3</v>
+        <v>3.4413063656696198E-2</v>
       </c>
       <c r="I39">
-        <v>6</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E40">
-        <v>55452.151259549602</v>
+        <v>6660.6410755234201</v>
       </c>
       <c r="F40">
-        <v>22391.905237149698</v>
+        <v>4243.5598320488398</v>
       </c>
       <c r="G40" s="1">
-        <v>0.44337112285077102</v>
+        <v>7.9120436533381702E-2</v>
       </c>
       <c r="H40" s="1">
-        <v>0.120148844843463</v>
+        <v>4.8422367063257803E-2</v>
       </c>
       <c r="I40">
-        <v>379</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -2111,22 +3606,25 @@
         <v>14</v>
       </c>
       <c r="E41">
-        <v>3567.1985905648598</v>
+        <v>2834.04994024594</v>
       </c>
       <c r="F41">
-        <v>1591.3059234979301</v>
+        <v>1252.1450061267799</v>
       </c>
       <c r="G41" s="1">
-        <v>2.8521758103263101E-2</v>
+        <v>2.72190987432816E-2</v>
       </c>
       <c r="H41" s="1">
-        <v>1.40511990210886E-2</v>
+        <v>1.38443517088659E-2</v>
       </c>
       <c r="I41">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I41">
+    <sortCondition ref="D1:D41"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>